<commit_message>
Interduced new Test for the Framework
Added:
Added Invalid Login Test, Add new First Address Test, product checkout
Test and search product Test
</commit_message>
<xml_diff>
--- a/testData/loginData.xlsx
+++ b/testData/loginData.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hi\eclipse-workspace\automation-assignment\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF3DAD6-3ECA-40E0-9F88-88AC511C01FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3837BD69-2733-4E8D-987F-C22D3042456F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>emailAddress</t>
   </si>
@@ -39,17 +35,34 @@
     <t>Password</t>
   </si>
   <si>
-    <t>jampani.kotaiahqa@gmail.com</t>
+    <t>bakomam596@skrak.com</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>Some Name</t>
+  </si>
+  <si>
+    <t>Jatin Sharma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,13 +85,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -357,43 +373,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.44140625" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{7DB56D4B-E1EB-472E-8D78-9DDF0AC6138B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>